<commit_message>
Adding in map functionality to app
</commit_message>
<xml_diff>
--- a/www/database.xlsx
+++ b/www/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852937AB-8498-4ABE-9E59-57585CF26B4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E53F97-B95E-4C0B-806C-B06888029D65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="459">
   <si>
     <t>Name</t>
   </si>
@@ -1075,11 +1075,6 @@
   </si>
   <si>
     <t>pets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   'has-drink': true,
-    'has-food': true,
-  },</t>
   </si>
   <si>
     <t>true</t>
@@ -1851,18 +1846,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AD105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AC105"/>
+    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="22" width="6" customWidth="1"/>
     <col min="29" max="29" width="90.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="72.81640625" customWidth="1"/>
+    <col min="30" max="30" width="5.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1944,16 +1939,14 @@
       <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="4" t="s">
-        <v>349</v>
-      </c>
+      <c r="AD1" s="4"/>
     </row>
     <row r="2" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D2" t="s">
         <v>141</v>
@@ -2013,10 +2006,10 @@
         <v>341</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC2" s="4" t="str">
         <f t="shared" ref="AC2:AC65" si="0">_xlfn.CONCAT("{
@@ -2029,13 +2022,17 @@
     'area': "old_town",'hours': {
       'sunday-start':"1600", 'sunday-end':"1800", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "", 'link':"https://acegilletts.com", 'pricing':"medium",   'phone-number': "", 'address': "239 South College Avenue, Fort Collins 80524", 'other-amenities': ['','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
+      <c r="AD2" t="str">
+        <f>CONCATENATE("Sunday:",H2,"-",I2)</f>
+        <v>Sunday:1600-1800</v>
+      </c>
     </row>
     <row r="3" spans="2:30" ht="120.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D3" t="s">
         <v>147</v>
@@ -2047,16 +2044,16 @@
         <v>148</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Z3" t="s">
         <v>28</v>
       </c>
       <c r="AA3" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB3" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC3" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2071,7 +2068,7 @@
         <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D4" t="s">
         <v>304</v>
@@ -2083,7 +2080,7 @@
         <v>150</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="X4" t="s">
         <v>338</v>
@@ -2095,10 +2092,10 @@
         <v>342</v>
       </c>
       <c r="AA4" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2113,7 +2110,7 @@
         <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D5" t="s">
         <v>66</v>
@@ -2170,7 +2167,7 @@
         <v>249</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="X5" t="s">
         <v>338</v>
@@ -2179,10 +2176,10 @@
         <v>341</v>
       </c>
       <c r="AA5" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB5" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2197,7 +2194,7 @@
         <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D6" t="s">
         <v>110</v>
@@ -2254,7 +2251,7 @@
         <v>258</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="X6" t="s">
         <v>338</v>
@@ -2263,10 +2260,10 @@
         <v>28</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB6" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2276,12 +2273,12 @@
       'sunday-start':"900", 'sunday-end':"2400", 'monday-start':"1100", 'monday-end':"2400", 'tuesday-start':"1100", 'tuesday-end':"2400", 'wednesday-start':"1100", 'wednesday-end':"2400", 'thursday-start':"1100", 'thursday-end':"2400", 'friday-start':"1100", 'friday-end':"2400", 'saturday-start':"900", 'saturday-end':"2400"},  'description': "Daily Specials", 'link':"http://www.avogadros.com", 'pricing':"medium",   'phone-number': "", 'address': "605 S Mason Street, Fort Collins 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="7" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:30" ht="116" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D7" t="s">
         <v>119</v>
@@ -2293,16 +2290,16 @@
         <v>108</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Z7" t="s">
         <v>28</v>
       </c>
       <c r="AA7" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB7" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2312,12 +2309,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.bannthairestaurant.net/", 'pricing':"low",   'phone-number': "", 'address': "626 S College Ave, Fort Collins 80524", 'other-amenities': ['','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="8" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:30" ht="145" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D8" t="s">
         <v>178</v>
@@ -2362,7 +2359,7 @@
         <v>272</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="X8" t="s">
         <v>338</v>
@@ -2371,10 +2368,10 @@
         <v>342</v>
       </c>
       <c r="AA8" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB8" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2384,12 +2381,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1600", 'monday-end':"1900", 'tuesday-start':"1600", 'tuesday-end':"1900", 'wednesday-start':"1600", 'wednesday-end':"1900", 'thursday-start':"1600", 'thursday-end':"1900", 'friday-start':"1600", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "$3.50 Drafts \n $4.50 Wines \n $5.50 Signature Martinis \n Half Price Select Apps and Flatbreads", 'link':"http://www.barlouie.com/locations/states/colorado/foothills-mall-fort-collins/", 'pricing':"medium",   'phone-number': "", 'address': "321 E Foothills Pkwy, Fort Collins, CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="9" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:30" ht="188.5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D9" t="s">
         <v>57</v>
@@ -2455,10 +2452,10 @@
         <v>28</v>
       </c>
       <c r="AA9" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB9" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2468,12 +2465,12 @@
       'sunday-start':"1500", 'sunday-end':"1800", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"1500", 'saturday-end':"1800"},  'description': "Everyday: $1 off Wells, Wines and Drafts \n Monday \n $1 off Domestic Bottles &amp; Drafts \n Tuesday \n $1 off Microbrews \n Wednesday \n $1 off all Gluten Free beer \n $3 Glass of House Wine \n Thursday \n $3 off Draft Pitchers \n $3 off Bottles of Wine \n Friday \n $6 Fat Tire Pints \n $3 Refills- Keep the Glass \n Saturday \n $3 Seasonal beers \n Sunday \n $3 Bloody Marys", 'link':"https://www.beaujos.com/", 'pricing':"medium",   'phone-number': "", 'address': "100 N College Ave, Fort Collins 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="10" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:30" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>256</v>
       </c>
       <c r="C10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D10" t="s">
         <v>106</v>
@@ -2530,16 +2527,16 @@
         <v>257</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Z10" t="s">
         <v>28</v>
       </c>
       <c r="AA10" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB10" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2549,12 +2546,12 @@
       'sunday-start':"1600", 'sunday-end':"2400", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"2400"},  'description': "Well Martini: $6.50 \n 100% Agave Margarita: $6.50 \n Draught Pine &amp; Bottled Beer: $1.00 off \n Wine by the Glass &amp; Well Drinks: $1.00 off \n Range of small bites and appetizers", 'link':"http://www.bigalsburgersanddogs.com/", 'pricing':"low",   'phone-number': "", 'address': "140 West Mountain Ave, Fort Collins 80524", 'other-amenities': ['','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="11" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:30" ht="116" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D11" t="s">
         <v>53</v>
@@ -2566,16 +2563,16 @@
         <v>55</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Z11" t="s">
         <v>28</v>
       </c>
       <c r="AA11" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2585,12 +2582,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.bigcityburrito.com/", 'pricing':"low",   'phone-number': "", 'address': "510 S College Ave, Fort Collins 80524", 'other-amenities': ['','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="12" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:30" ht="145" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>344</v>
       </c>
       <c r="C12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D12" t="s">
         <v>78</v>
@@ -2641,10 +2638,10 @@
         <v>342</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB12" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC12" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2654,12 +2651,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1900", 'tuesday-start':"1500", 'tuesday-end':"1900", 'wednesday-start':"1500", 'wednesday-end':"1900", 'thursday-start':"1500", 'thursday-end':"1900", 'friday-start':"1500", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "$2 Domestic Bottles \n $3 Wine \n $4 Calls \n $1 off draft beer and cocktails \n 1/2 off most apps and mini pizzas", 'link':"https://www.bjsrestaurants.com/locations/co/fort-collins", 'pricing':"medium",   'phone-number': "", 'address': "2670 E Harmony Rd, Fort Collins, CO 80525", 'other-amenities': ['','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="13" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:30" ht="145" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D13" t="s">
         <v>304</v>
@@ -2725,10 +2722,10 @@
         <v>342</v>
       </c>
       <c r="AA13" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB13" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2738,12 +2735,12 @@
       'sunday-start':"1100", 'sunday-end':"1600", 'monday-start':"1100", 'monday-end':"1600", 'tuesday-start':"1100", 'tuesday-end':"1600", 'wednesday-start':"1100", 'wednesday-end':"1600", 'thursday-start':"1100", 'thursday-end':"1600", 'friday-start':"1100", 'friday-end':"1600", 'saturday-start':"1100", 'saturday-end':"1600"},  'description': "$1 off Black Bottle Beers \n $4 well drinks", 'link':"https://blackbottleCraft Beer.com/", 'pricing':"medium",   'phone-number': "", 'address': "1611 S. College Ave., Ste 1609, Fort Collins, CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="14" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:30" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>291</v>
       </c>
       <c r="C14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D14" t="s">
         <v>78</v>
@@ -2794,16 +2791,16 @@
         <v>292</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Z14" t="s">
         <v>341</v>
       </c>
       <c r="AA14" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB14" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2813,12 +2810,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1000", 'monday-end':"1400", 'tuesday-start':"1400", 'tuesday-end':"1900", 'wednesday-start':"1400", 'wednesday-end':"1900", 'thursday-start':"1400", 'thursday-end':"1900", 'friday-start':"1400", 'friday-end':"1900", 'saturday-start':"1100", 'saturday-end':"1600"},  'description': "Tues-Fri: \n $3 select micros \n $2.50 domestics \n $3 wells \n $4 wine \n $5-7 select appetizers \n Saturdays: \n $12 select micro pitchers \n $10 domestic pitchers \n $3 select cocktails \n $1 mimosas \n $5 build your own bloody mary bar \n $14 all you can eat brunch. ", 'link':"http://www.blindpigfortcollins.com/", 'pricing':"medium",   'phone-number': "", 'address': "214 Linden St, Fort Collins, CO 80524", 'other-amenities': ['','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="15" spans="2:30" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:30" ht="145" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D15" t="s">
         <v>53</v>
@@ -2863,7 +2860,7 @@
         <v>293</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="X15" t="s">
         <v>338</v>
@@ -2872,10 +2869,10 @@
         <v>341</v>
       </c>
       <c r="AA15" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB15" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2890,7 +2887,7 @@
         <v>294</v>
       </c>
       <c r="C16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D16" t="s">
         <v>78</v>
@@ -2926,10 +2923,10 @@
         <v>341</v>
       </c>
       <c r="AA16" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB16" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2944,7 +2941,7 @@
         <v>182</v>
       </c>
       <c r="C17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D17" t="s">
         <v>78</v>
@@ -2956,16 +2953,16 @@
         <v>183</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Z17" t="s">
         <v>342</v>
       </c>
       <c r="AA17" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB17" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2975,12 +2972,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.buffalowildwings.com", 'pricing':"low",   'phone-number': "", 'address': "150 E. Harmony Road, 2A, Fort Collins, CO 80525", 'other-amenities': ['','','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="18" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D18" t="s">
         <v>71</v>
@@ -2992,7 +2989,7 @@
         <v>72</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="X18" t="s">
         <v>338</v>
@@ -3001,10 +2998,10 @@
         <v>28</v>
       </c>
       <c r="AA18" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB18" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3014,12 +3011,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.cafevino.com/", 'pricing':"medium",   'phone-number': "", 'address': "1200 S College Ave., Fort Collins 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="19" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:29" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D19" t="s">
         <v>53</v>
@@ -3028,55 +3025,55 @@
         <v>28</v>
       </c>
       <c r="G19" t="s">
+        <v>443</v>
+      </c>
+      <c r="H19">
+        <v>1600</v>
+      </c>
+      <c r="I19">
+        <v>1800</v>
+      </c>
+      <c r="J19">
+        <v>1600</v>
+      </c>
+      <c r="K19">
+        <v>1800</v>
+      </c>
+      <c r="L19">
+        <v>1600</v>
+      </c>
+      <c r="M19">
+        <v>1800</v>
+      </c>
+      <c r="N19">
+        <v>1600</v>
+      </c>
+      <c r="O19">
+        <v>1800</v>
+      </c>
+      <c r="P19">
+        <v>1600</v>
+      </c>
+      <c r="Q19">
+        <v>1800</v>
+      </c>
+      <c r="R19">
+        <v>1600</v>
+      </c>
+      <c r="S19">
+        <v>1800</v>
+      </c>
+      <c r="T19">
+        <v>1600</v>
+      </c>
+      <c r="U19">
+        <v>1800</v>
+      </c>
+      <c r="V19" t="s">
         <v>444</v>
       </c>
-      <c r="H19">
-        <v>1600</v>
-      </c>
-      <c r="I19">
-        <v>1800</v>
-      </c>
-      <c r="J19">
-        <v>1600</v>
-      </c>
-      <c r="K19">
-        <v>1800</v>
-      </c>
-      <c r="L19">
-        <v>1600</v>
-      </c>
-      <c r="M19">
-        <v>1800</v>
-      </c>
-      <c r="N19">
-        <v>1600</v>
-      </c>
-      <c r="O19">
-        <v>1800</v>
-      </c>
-      <c r="P19">
-        <v>1600</v>
-      </c>
-      <c r="Q19">
-        <v>1800</v>
-      </c>
-      <c r="R19">
-        <v>1600</v>
-      </c>
-      <c r="S19">
-        <v>1800</v>
-      </c>
-      <c r="T19">
-        <v>1600</v>
-      </c>
-      <c r="U19">
-        <v>1800</v>
-      </c>
-      <c r="V19" t="s">
-        <v>445</v>
-      </c>
       <c r="W19" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="X19" t="s">
         <v>338</v>
@@ -3085,10 +3082,10 @@
         <v>342</v>
       </c>
       <c r="AA19" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB19" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3098,7 +3095,7 @@
       'sunday-start':"1600", 'sunday-end':"1800", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "Frozen Lime Margarita: $4 \n Frozen Mango Margarita: $6 \n Coin Margarita: $5 \n Coors Light: $4 \n Tecate: $4 \n Wine: $5 \n Street Tacos: $2 for 1, $5 for 3, $8 for 5 \n Wide Selection of Happy Hour Foods", 'link':"http://matadorrestaurants.com/mexican-food-fort-collins", 'pricing':"medium",   'phone-number': "", 'address': "341 E Foothills Pkwy #110 Fort Collins, CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="20" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>307</v>
       </c>
@@ -3163,10 +3160,10 @@
         <v>342</v>
       </c>
       <c r="AA20" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB20" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3181,7 +3178,7 @@
         <v>306</v>
       </c>
       <c r="C21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D21" t="s">
         <v>78</v>
@@ -3235,10 +3232,10 @@
         <v>342</v>
       </c>
       <c r="AA21" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB21" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3248,12 +3245,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "$4 drafts \n $4.50 wells \n $6 wine", 'link':"https://www.cbpotts.com/locations/foothills/", 'pricing':"medium",   'phone-number': "", 'address': "195 E Foothills Parkway, Fort Collins CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="22" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D22" t="s">
         <v>90</v>
@@ -3274,10 +3271,10 @@
         <v>28</v>
       </c>
       <c r="AA22" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB22" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC22" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3292,7 +3289,7 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -3322,10 +3319,10 @@
         <v>341</v>
       </c>
       <c r="AA23" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB23" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3340,7 +3337,7 @@
         <v>153</v>
       </c>
       <c r="C24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D24" t="s">
         <v>154</v>
@@ -3352,16 +3349,16 @@
         <v>155</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Z24" t="s">
         <v>28</v>
       </c>
       <c r="AA24" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB24" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3376,7 +3373,7 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -3433,10 +3430,10 @@
         <v>28</v>
       </c>
       <c r="AA25" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB25" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC25" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3446,12 +3443,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "Mugs: $2.75 \n 20 Ounce Pints: $4 \n Pitchers: $12 \n Bargain Priced Pool", 'link':"https://coopersmithspub.com", 'pricing':"medium",   'phone-number': "", 'address': "5 Old Town Sq, Fort Collins 80524", 'other-amenities': ['outdoor','pets','medium'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="26" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>156</v>
       </c>
       <c r="C26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D26" t="s">
         <v>157</v>
@@ -3484,7 +3481,7 @@
         <v>299</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="X26" t="s">
         <v>338</v>
@@ -3493,10 +3490,10 @@
         <v>28</v>
       </c>
       <c r="AA26" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB26" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC26" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3506,12 +3503,12 @@
       'sunday-start':"1200", 'sunday-end':"1900", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"1600", 'wednesday-end':"2100", 'thursday-start':"1600", 'thursday-end':"2100", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "Sundays: $2 off Bloody Mary’s \n Wed-Thur: \n $6 select cocktails including mules \n $2 off select appetizers", 'link':"http://www.coppermuse.com/", 'pricing':"medium",   'phone-number': "", 'address': "244 N. College Ave, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="27" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D27" t="s">
         <v>78</v>
@@ -3568,7 +3565,7 @@
         <v>250</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="X27" t="s">
         <v>338</v>
@@ -3577,10 +3574,10 @@
         <v>28</v>
       </c>
       <c r="AA27" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB27" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3595,7 +3592,7 @@
         <v>185</v>
       </c>
       <c r="C28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D28" t="s">
         <v>186</v>
@@ -3646,10 +3643,10 @@
         <v>342</v>
       </c>
       <c r="AA28" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB28" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC28" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3659,12 +3656,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "", 'link':"https://www.domenicsrestaurant.com", 'pricing':"medium",   'phone-number': "", 'address': "931 E. Harmony Road, Fort Collins Shopping Cener, Fort Collins, CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="29" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D29" t="s">
         <v>87</v>
@@ -3676,16 +3673,16 @@
         <v>88</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Z29" t="s">
         <v>342</v>
       </c>
       <c r="AA29" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB29" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC29" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3700,7 +3697,7 @@
         <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D30" t="s">
         <v>69</v>
@@ -3712,16 +3709,16 @@
         <v>70</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Z30" t="s">
         <v>342</v>
       </c>
       <c r="AA30" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB30" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC30" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3736,7 +3733,7 @@
         <v>159</v>
       </c>
       <c r="C31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D31" t="s">
         <v>160</v>
@@ -3748,7 +3745,7 @@
         <v>161</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="X31" t="s">
         <v>338</v>
@@ -3757,10 +3754,10 @@
         <v>342</v>
       </c>
       <c r="AA31" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB31" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC31" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3775,7 +3772,7 @@
         <v>300</v>
       </c>
       <c r="C32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D32" t="s">
         <v>226</v>
@@ -3820,16 +3817,16 @@
         <v>301</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Z32" t="s">
         <v>341</v>
       </c>
       <c r="AA32" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB32" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC32" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3839,78 +3836,78 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1630", 'monday-end':"1900", 'tuesday-start':"1630", 'tuesday-end':"1900", 'wednesday-start':"1630", 'wednesday-end':"1900", 'thursday-start':"1630", 'thursday-end':"1900", 'friday-start':"1630", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "$2 off martinis \n $2 off tapas", 'link':"http://www.elliotsmartini.com/", 'pricing':"medium",   'phone-number': "", 'address': "234 Linden St, Fort Collins, CO 80524", 'other-amenities': ['','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="33" spans="2:29" ht="131.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:29" ht="160.5" x14ac:dyDescent="0.45">
       <c r="B33" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="C33" t="s">
+        <v>351</v>
+      </c>
+      <c r="D33" t="s">
+        <v>419</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="C33" t="s">
-        <v>352</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="H33">
+        <v>1500</v>
+      </c>
+      <c r="I33">
+        <v>1800</v>
+      </c>
+      <c r="J33">
+        <v>1500</v>
+      </c>
+      <c r="K33">
+        <v>1800</v>
+      </c>
+      <c r="L33">
+        <v>1500</v>
+      </c>
+      <c r="M33">
+        <v>1800</v>
+      </c>
+      <c r="N33">
+        <v>1500</v>
+      </c>
+      <c r="O33">
+        <v>1800</v>
+      </c>
+      <c r="P33">
+        <v>1500</v>
+      </c>
+      <c r="Q33">
+        <v>1800</v>
+      </c>
+      <c r="R33">
+        <v>1500</v>
+      </c>
+      <c r="S33">
+        <v>1800</v>
+      </c>
+      <c r="T33">
+        <v>1500</v>
+      </c>
+      <c r="U33">
+        <v>1800</v>
+      </c>
+      <c r="V33" t="s">
+        <v>421</v>
+      </c>
+      <c r="W33" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="E33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="H33">
-        <v>1500</v>
-      </c>
-      <c r="I33">
-        <v>1800</v>
-      </c>
-      <c r="J33">
-        <v>1500</v>
-      </c>
-      <c r="K33">
-        <v>1800</v>
-      </c>
-      <c r="L33">
-        <v>1500</v>
-      </c>
-      <c r="M33">
-        <v>1800</v>
-      </c>
-      <c r="N33">
-        <v>1500</v>
-      </c>
-      <c r="O33">
-        <v>1800</v>
-      </c>
-      <c r="P33">
-        <v>1500</v>
-      </c>
-      <c r="Q33">
-        <v>1800</v>
-      </c>
-      <c r="R33">
-        <v>1500</v>
-      </c>
-      <c r="S33">
-        <v>1800</v>
-      </c>
-      <c r="T33">
-        <v>1500</v>
-      </c>
-      <c r="U33">
-        <v>1800</v>
-      </c>
-      <c r="V33" t="s">
-        <v>422</v>
-      </c>
-      <c r="W33" s="2" t="s">
-        <v>421</v>
-      </c>
       <c r="Z33" t="s">
         <v>28</v>
       </c>
       <c r="AA33" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB33" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC33" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3920,12 +3917,12 @@
       'sunday-start':"1500", 'sunday-end':"1800", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"1500", 'saturday-end':"1800"},  'description': "Aperol Spritz, Gin and Tonic, Martini, Manhattan, Local Draft Beer, French 75, Negroni, Old Fashioned: $5 \n House Red Wine, House White Wine, Rose of the Day: $6 \n Selection of Happy Hour Foods", 'link':"http://emporiumftcollins.com/", 'pricing':"medium",   'phone-number': "", 'address': "378 Walnut St, Fort Collins, CO 80524", 'other-amenities': ['','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="34" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>275</v>
       </c>
       <c r="C34" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D34" t="s">
         <v>188</v>
@@ -3937,16 +3934,16 @@
         <v>189</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="Z34" t="s">
         <v>342</v>
       </c>
       <c r="AA34" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB34" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC34" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3956,12 +3953,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.feistyspirits.com/", 'pricing':"medium",   'phone-number': "", 'address': "1708 East Lincoln Ave. #1, Fort Collins, CO 80524", 'other-amenities': ['','','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="35" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D35" t="s">
         <v>93</v>
@@ -4018,16 +4015,16 @@
         <v>255</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Z35" t="s">
         <v>28</v>
       </c>
       <c r="AA35" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB35" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC35" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4037,12 +4034,12 @@
       'sunday-start':"1600", 'sunday-end':"1800", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"1500", 'saturday-end':"1800"},  'description': "Extensive menu of discounted &amp; Happy Hour only food items as well as sixteen different half price wines and discounts on draft beer and cocktails", 'link':"http://www.fishmkt.com", 'pricing':"high",   'phone-number': "", 'address': "150 W Oak Street, Fort Collins 80524", 'other-amenities': ['','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="36" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D36" t="s">
         <v>75</v>
@@ -4054,16 +4051,16 @@
         <v>76</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Z36" t="s">
         <v>342</v>
       </c>
       <c r="AA36" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB36" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC36" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4073,12 +4070,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.fiveguys.com/", 'pricing':"Low",   'phone-number': "", 'address': "1335 W Elizabeth St, Fort Collins 80521", 'other-amenities': ['','','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="37" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>302</v>
       </c>
       <c r="C37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D37" t="s">
         <v>303</v>
@@ -4135,7 +4132,7 @@
         <v>308</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="X37" t="s">
         <v>338</v>
@@ -4144,10 +4141,10 @@
         <v>341</v>
       </c>
       <c r="AA37" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB37" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC37" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4157,12 +4154,12 @@
       'sunday-start':"1400", 'sunday-end':"2200", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "$2 off select drafts ", 'link':"http://www.theforgepublickhouse.com", 'pricing':"medium",   'phone-number': "", 'address': "255 Old Firehouse Alley, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="38" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>310</v>
       </c>
       <c r="C38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D38" t="s">
         <v>186</v>
@@ -4207,16 +4204,16 @@
         <v>311</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Z38" t="s">
         <v>342</v>
       </c>
       <c r="AA38" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB38" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC38" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4231,7 +4228,7 @@
         <v>190</v>
       </c>
       <c r="C39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D39" t="s">
         <v>53</v>
@@ -4249,10 +4246,10 @@
         <v>28</v>
       </c>
       <c r="AA39" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB39" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC39" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4267,7 +4264,7 @@
         <v>192</v>
       </c>
       <c r="C40" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D40" t="s">
         <v>53</v>
@@ -4285,10 +4282,10 @@
         <v>342</v>
       </c>
       <c r="AA40" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB40" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC40" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4303,7 +4300,7 @@
         <v>194</v>
       </c>
       <c r="C41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D41" t="s">
         <v>303</v>
@@ -4324,10 +4321,10 @@
         <v>342</v>
       </c>
       <c r="AA41" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB41" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC41" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4342,7 +4339,7 @@
         <v>313</v>
       </c>
       <c r="C42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D42" t="s">
         <v>303</v>
@@ -4393,16 +4390,16 @@
         <v>314</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Z42" t="s">
         <v>341</v>
       </c>
       <c r="AA42" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB42" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC42" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4414,55 +4411,55 @@
     </row>
     <row r="43" spans="2:29" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C43" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D43" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E43" t="s">
         <v>28</v>
       </c>
       <c r="G43" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="H43">
+        <v>1600</v>
+      </c>
+      <c r="I43">
+        <v>1800</v>
+      </c>
+      <c r="J43">
+        <v>1600</v>
+      </c>
+      <c r="K43">
+        <v>1800</v>
+      </c>
+      <c r="L43">
+        <v>1600</v>
+      </c>
+      <c r="M43">
+        <v>1800</v>
+      </c>
+      <c r="N43">
+        <v>1600</v>
+      </c>
+      <c r="O43">
+        <v>1800</v>
+      </c>
+      <c r="P43">
+        <v>1600</v>
+      </c>
+      <c r="Q43">
+        <v>1800</v>
+      </c>
+      <c r="V43" t="s">
+        <v>440</v>
+      </c>
+      <c r="W43" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="H43">
-        <v>1600</v>
-      </c>
-      <c r="I43">
-        <v>1800</v>
-      </c>
-      <c r="J43">
-        <v>1600</v>
-      </c>
-      <c r="K43">
-        <v>1800</v>
-      </c>
-      <c r="L43">
-        <v>1600</v>
-      </c>
-      <c r="M43">
-        <v>1800</v>
-      </c>
-      <c r="N43">
-        <v>1600</v>
-      </c>
-      <c r="O43">
-        <v>1800</v>
-      </c>
-      <c r="P43">
-        <v>1600</v>
-      </c>
-      <c r="Q43">
-        <v>1800</v>
-      </c>
-      <c r="V43" t="s">
-        <v>441</v>
-      </c>
-      <c r="W43" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="X43" t="s">
         <v>338</v>
@@ -4471,10 +4468,10 @@
         <v>342</v>
       </c>
       <c r="AA43" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB43" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC43" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4489,7 +4486,7 @@
         <v>196</v>
       </c>
       <c r="C44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D44" t="s">
         <v>303</v>
@@ -4501,7 +4498,7 @@
         <v>197</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="X44" t="s">
         <v>338</v>
@@ -4513,10 +4510,10 @@
         <v>28</v>
       </c>
       <c r="AA44" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB44" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC44" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4526,12 +4523,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.horseanddragonbrewing.com/", 'pricing':"medium",   'phone-number': "", 'address': "124 Racquette Drive, Fort Collins, CO 80524", 'other-amenities': ['outdoor','pets','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="45" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D45" t="s">
         <v>47</v>
@@ -4549,10 +4546,10 @@
         <v>341</v>
       </c>
       <c r="AA45" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB45" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC45" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4562,12 +4559,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.huhot.com/", 'pricing':"medium",   'phone-number': "", 'address': "249 S College Ave, Fort Collins 80524", 'other-amenities': ['','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="46" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:29" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>162</v>
       </c>
       <c r="C46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D46" t="s">
         <v>53</v>
@@ -4624,7 +4621,7 @@
         <v>316</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="X46" t="s">
         <v>338</v>
@@ -4633,10 +4630,10 @@
         <v>341</v>
       </c>
       <c r="AA46" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB46" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC46" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4646,12 +4643,12 @@
       'sunday-start':"1500", 'sunday-end':"2000", 'monday-start':"1500", 'monday-end':"2000", 'tuesday-start':"1500", 'tuesday-end':"2000", 'wednesday-start':"1500", 'wednesday-end':"2000", 'thursday-start':"1500", 'thursday-end':"2000", 'friday-start':"1500", 'friday-end':"2000", 'saturday-start':"1500", 'saturday-end':"2000"},  'description': "$2.50 Coors Lights &amp; Coors Drafts \n $3.50 Select Craft Drafts \n $4 House Margaritas \n $3 Wells \n Free Chips and Salsa w/ Bar purchase", 'link':"http://www.illegalpetes.com/fort-collins-old-town", 'pricing':"low",   'phone-number': "", 'address': "320 Walnut Street, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="47" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>198</v>
       </c>
       <c r="C47" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D47" t="s">
         <v>303</v>
@@ -4663,16 +4660,16 @@
         <v>199</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Z47" t="s">
         <v>342</v>
       </c>
       <c r="AA47" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB47" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC47" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4682,12 +4679,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.intersectbrewing.com/", 'pricing':"medium",   'phone-number': "", 'address': "2160 W. Drake Road, Fort Collins, CO 80526", 'other-amenities': ['','','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="48" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D48" t="s">
         <v>135</v>
@@ -4744,16 +4741,16 @@
         <v>263</v>
       </c>
       <c r="W48" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="Z48" t="s">
         <v>342</v>
       </c>
       <c r="AA48" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB48" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC48" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4763,12 +4760,12 @@
       'sunday-start':"1500", 'sunday-end':"1900", 'monday-start':"1500", 'monday-end':"1900", 'tuesday-start':"1500", 'tuesday-end':"1900", 'wednesday-start':"1500", 'wednesday-end':"1900", 'thursday-start':"1500", 'thursday-end':"1900", 'friday-start':"1500", 'friday-end':"1900", 'saturday-start':"1500", 'saturday-end':"1900"},  'description': "$3.25 Domestic Pints \n $3.00 Shot Specials \n $3.50 Well Drinks \n $4.25 Micro Beer Pints \n $4.00 House Wines \n $5.00 Margaritas \n $6.00 House Martinis", 'link':"http://www.islandgrillrestaurant.com", 'pricing':"medium",   'phone-number': "", 'address': "2601 S Lemay Ave Unit 12, Fort Collins 80525", 'other-amenities': ['','','easy'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="49" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D49" t="s">
         <v>93</v>
@@ -4834,10 +4831,10 @@
         <v>341</v>
       </c>
       <c r="AA49" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB49" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC49" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4847,12 +4844,12 @@
       'sunday-start':"1600", 'sunday-end':"1800", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "Numerous food and drink specials including a wide selection of oysters, mussels, and shrimp", 'link':"https://www.jaxfishhouse.com/fort-collins/", 'pricing':"high",   'phone-number': "", 'address': "123 N College Ave., Fort Collins, CO, Fort Collins 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="50" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D50" t="s">
         <v>34</v>
@@ -4918,10 +4915,10 @@
         <v>341</v>
       </c>
       <c r="AA50" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB50" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC50" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4931,12 +4928,12 @@
       'sunday-start':"1500", 'sunday-end':"1830", 'monday-start':"1500", 'monday-end':"1830", 'tuesday-start':"1500", 'tuesday-end':"1830", 'wednesday-start':"1500", 'wednesday-end':"1830", 'thursday-start':"1500", 'thursday-end':"1830", 'friday-start':"1500", 'friday-end':"1830", 'saturday-start':"1500", 'saturday-end':"1830"},  'description': "Cocktails: $5 \n Martinis: $6 \n Wine by the Glass: $5 \n Selected Draft Beers: $3.50", 'link':"http://www.jaysbistro.net/", 'pricing':"high",   'phone-number': "", 'address': "135 W Oak St, Fort Collins 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="51" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:29" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>115</v>
       </c>
       <c r="C51" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D51" t="s">
         <v>116</v>
@@ -4951,7 +4948,7 @@
         <v>259</v>
       </c>
       <c r="W51" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="X51" t="s">
         <v>338</v>
@@ -4960,10 +4957,10 @@
         <v>28</v>
       </c>
       <c r="AA51" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB51" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC51" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4973,12 +4970,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "House Hot Sake $2.50 (small) $5.00 (large) \n House Wine $5.00 \n Sake Bomb $2.00 \n ODELL IPA (FT. COLLINS) $3.00 \n Kirin Ichiban (draft) $3.00 \n New Belgium (draft) $3.00 \n Corona (bottle) $2.50 \n Coors Light (bottle) $2.50 \n Bud Light (bottle) $2.50 \n Wide range of sushi specials", 'link':"http://www.sushijeju.com", 'pricing':"medium",   'phone-number': "", 'address': "238 S College Ave, Fort Collins 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="52" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D52" t="s">
         <v>132</v>
@@ -4990,16 +4987,16 @@
         <v>133</v>
       </c>
       <c r="W52" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Z52" t="s">
         <v>28</v>
       </c>
       <c r="AA52" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB52" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC52" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5009,12 +5006,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.jimswings.com/", 'pricing':"low",   'phone-number': "", 'address': "1205 W Elizabeth St Ste C, Fort Collins 80521", 'other-amenities': ['','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="53" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D53" t="s">
         <v>96</v>
@@ -5026,16 +5023,16 @@
         <v>97</v>
       </c>
       <c r="W53" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Z53" t="s">
         <v>342</v>
       </c>
       <c r="AA53" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB53" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC53" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5050,7 +5047,7 @@
         <v>164</v>
       </c>
       <c r="C54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D54" t="s">
         <v>53</v>
@@ -5089,7 +5086,7 @@
         <v>267</v>
       </c>
       <c r="W54" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="X54" t="s">
         <v>338</v>
@@ -5098,10 +5095,10 @@
         <v>341</v>
       </c>
       <c r="AA54" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB54" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC54" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5111,21 +5108,21 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "$3 Shots and Drafts \n $5 Jefe, Del Sol, Pomegranate Marg, MND &amp; Lunch Box", 'link':"http://www.laluzgrill.com", 'pricing':"medium",   'phone-number': "", 'address': "200 Walnut Street, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="55" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
+        <v>427</v>
+      </c>
+      <c r="C55" t="s">
+        <v>353</v>
+      </c>
+      <c r="D55" t="s">
         <v>428</v>
       </c>
-      <c r="C55" t="s">
-        <v>354</v>
-      </c>
-      <c r="D55" t="s">
-        <v>429</v>
-      </c>
       <c r="E55" t="s">
         <v>28</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H55">
         <v>1600</v>
@@ -5164,19 +5161,19 @@
         <v>1900</v>
       </c>
       <c r="V55" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="W55" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Z55" t="s">
         <v>342</v>
       </c>
       <c r="AA55" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB55" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC55" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5186,12 +5183,12 @@
       'sunday-start':"1600", 'sunday-end':"1900", 'monday-start':"1600", 'monday-end':"1900", 'tuesday-start':"1600", 'tuesday-end':"1900", 'wednesday-start':"1600", 'wednesday-end':"1900", 'thursday-start':"1600", 'thursday-end':"1900", 'friday-start':"1600", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "Cocktails: $5 \n Wine: $4 \n Domestic Drafts: $3 \n Chili Cheese Fries: $5 \n Spicy Chicken Bites: $4 \n Fried Pickles: $3", 'link':"https://www.longhornsteakhouse.com/home", 'pricing':"medium",   'phone-number': "", 'address': " 3450 S College Ave, Fort Collins, CO 80525", 'other-amenities': ['','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="56" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:29" ht="174" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>200</v>
       </c>
       <c r="C56" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D56" t="s">
         <v>53</v>
@@ -5248,7 +5245,7 @@
         <v>337</v>
       </c>
       <c r="W56" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="X56" t="s">
         <v>338</v>
@@ -5257,10 +5254,10 @@
         <v>28</v>
       </c>
       <c r="AA56" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB56" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC56" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5270,12 +5267,12 @@
       'sunday-start':"1100", 'sunday-end':"2200", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1100", 'tuesday-end':"1730", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "House Margaritas $8.00 \n Gold House Pitcher $17.00 \n​ Classic Margaritas $4.25 \n Classic Pitchers $19 \n Imported Beer $2 \n Domestic Beer $2 \n Tuesdays - Lady's Day (all day) \n Sunday - Men's Day (all day) \n 2 for 1 on House Margs, Classic Margs, Beers, and Wines \n Wed - Buy a Pitcher and Get a Free App 11am-4pm &amp; 6pm-10pm", 'link':"http://www.lostaracos.com", 'pricing':"medium",   'phone-number': "", 'address': "626 S College Ave, Fort Collins 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="57" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:29" ht="188.5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>318</v>
       </c>
       <c r="C57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D57" t="s">
         <v>319</v>
@@ -5332,16 +5329,16 @@
         <v>320</v>
       </c>
       <c r="W57" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Z57" t="s">
         <v>341</v>
       </c>
       <c r="AA57" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB57" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC57" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5351,24 +5348,24 @@
       'sunday-start':"1100", 'sunday-end':"2400", 'monday-start':"1500", 'monday-end':"1900", 'tuesday-start':"1500", 'tuesday-end':"1900", 'wednesday-start':"1500", 'wednesday-end':"1900", 'thursday-start':"1500", 'thursday-end':"1900", 'friday-start':"1500", 'friday-end':"1900", 'saturday-start':"1100", 'saturday-end':"1900"},  'description': "Monday-Friday \n $1 off wells, wines, and drafts \n Saturday \n $1.50 Bud and Coors \n $2.50 wells and micros \n $3.50 Guinness \n $1 off wines \n Monday \n $3.50 burger baskets \n $2.50 pints of 90 Schilling, 5 Barrel, Odell IPA \n Tuesday \n $2.50 Guinness pints all day \n Wednesday \n $2.50 You Call It 7pm-close \n Thursday \n $3 pints w/ $3 bomb shots \n Sunday \n $2 Bloody Marys, well vodka drinks, and green chili \n $2.50 New Belgium", 'link':"http://www.luckyjoes.com/", 'pricing':"medium",   'phone-number': "", 'address': "25 Old Town Square, Fort Collins, CO 80524", 'other-amenities': ['','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="58" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
+        <v>422</v>
+      </c>
+      <c r="C58" t="s">
+        <v>351</v>
+      </c>
+      <c r="D58" t="s">
         <v>423</v>
       </c>
-      <c r="C58" t="s">
-        <v>352</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="W58" t="s">
         <v>424</v>
-      </c>
-      <c r="E58" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="W58" t="s">
-        <v>425</v>
       </c>
       <c r="X58" t="s">
         <v>338</v>
@@ -5377,10 +5374,10 @@
         <v>28</v>
       </c>
       <c r="AA58" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB58" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC58" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5390,12 +5387,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://magicratlivemusic.com", 'pricing':"medium",   'phone-number': "", 'address': "378 Walnut St, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="59" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>322</v>
       </c>
       <c r="C59" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D59" t="s">
         <v>323</v>
@@ -5452,16 +5449,16 @@
         <v>324</v>
       </c>
       <c r="W59" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Z59" t="s">
         <v>341</v>
       </c>
       <c r="AA59" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB59" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC59" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5476,7 +5473,7 @@
         <v>166</v>
       </c>
       <c r="C60" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D60" t="s">
         <v>303</v>
@@ -5488,7 +5485,7 @@
         <v>167</v>
       </c>
       <c r="W60" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="X60" t="s">
         <v>338</v>
@@ -5500,10 +5497,10 @@
         <v>342</v>
       </c>
       <c r="AA60" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB60" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC60" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5513,12 +5510,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.maxlinebrewing.com", 'pricing':"low",   'phone-number': "", 'address': "2724 McClelland Drive Unit 190, Fort Collins, CO 80525", 'other-amenities': ['outdoor','pets','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="61" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -5536,10 +5533,10 @@
         <v>28</v>
       </c>
       <c r="AA61" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB61" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC61" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5549,12 +5546,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.meltingpot.com/fort-collins-co/", 'pricing':"high",   'phone-number': "", 'address': "334 E Mountain Ave, Fort Collins 80524", 'other-amenities': ['','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="62" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D62" t="s">
         <v>188</v>
@@ -5566,16 +5563,16 @@
         <v>202</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Z62" t="s">
         <v>28</v>
       </c>
       <c r="AA62" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB62" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC62" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5587,10 +5584,10 @@
     </row>
     <row r="63" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D63" t="s">
         <v>132</v>
@@ -5599,10 +5596,10 @@
         <v>28</v>
       </c>
       <c r="G63" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="W63" t="s">
         <v>452</v>
-      </c>
-      <c r="W63" t="s">
-        <v>453</v>
       </c>
       <c r="X63" t="s">
         <v>338</v>
@@ -5611,10 +5608,10 @@
         <v>28</v>
       </c>
       <c r="AA63" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB63" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC63" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5624,12 +5621,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.moesoriginalbbq.com/lo/fort-collins", 'pricing':"medium",   'phone-number': "", 'address': "181 N College Ave", 'other-amenities': ['outdoor','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="64" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>121</v>
       </c>
       <c r="C64" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D64" t="s">
         <v>104</v>
@@ -5686,7 +5683,7 @@
         <v>260</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="X64" t="s">
         <v>338</v>
@@ -5695,10 +5692,10 @@
         <v>342</v>
       </c>
       <c r="AA64" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB64" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC64" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5713,7 +5710,7 @@
         <v>168</v>
       </c>
       <c r="C65" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D65" t="s">
         <v>154</v>
@@ -5770,16 +5767,16 @@
         <v>268</v>
       </c>
       <c r="W65" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Z65" t="s">
         <v>342</v>
       </c>
       <c r="AA65" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB65" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC65" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5794,7 +5791,7 @@
         <v>203</v>
       </c>
       <c r="C66" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D66" t="s">
         <v>303</v>
@@ -5806,7 +5803,7 @@
         <v>204</v>
       </c>
       <c r="W66" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="X66" t="s">
         <v>338</v>
@@ -5818,10 +5815,10 @@
         <v>28</v>
       </c>
       <c r="AA66" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB66" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC66" s="4" t="str">
         <f t="shared" ref="AC66:AC105" si="1">_xlfn.CONCAT("{
@@ -5840,7 +5837,7 @@
         <v>170</v>
       </c>
       <c r="C67" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D67" t="s">
         <v>57</v>
@@ -5879,7 +5876,7 @@
         <v>270</v>
       </c>
       <c r="W67" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="X67" t="s">
         <v>338</v>
@@ -5888,10 +5885,10 @@
         <v>342</v>
       </c>
       <c r="AA67" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB67" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC67" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5901,12 +5898,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1530", 'monday-end':"1800", 'tuesday-start':"1530", 'tuesday-end':"1800", 'wednesday-start':"1530", 'wednesday-end':"1800", 'thursday-start':"1530", 'thursday-end':"1800", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "Draft beers $3.00 \n Budwiser $2.00 \n House Wine $3.75 \n Appetizer specials and pizza by the slice", 'link':"http://www.nicksfc.com/", 'pricing':"medium",   'phone-number': "", 'address': "1100 S. College Avenue, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="68" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>123</v>
       </c>
       <c r="C68" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D68" t="s">
         <v>124</v>
@@ -5924,10 +5921,10 @@
         <v>342</v>
       </c>
       <c r="AA68" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB68" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC68" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5942,7 +5939,7 @@
         <v>205</v>
       </c>
       <c r="C69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D69" t="s">
         <v>303</v>
@@ -5966,10 +5963,10 @@
         <v>28</v>
       </c>
       <c r="AA69" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB69" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC69" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5979,12 +5976,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.odellbrewing.com/", 'pricing':"medium",   'phone-number': "", 'address': "800 E. Lincoln Avenue, Fort Collins, CO 80524", 'other-amenities': ['outdoor','pets','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="70" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D70" t="s">
         <v>144</v>
@@ -6002,10 +5999,10 @@
         <v>341</v>
       </c>
       <c r="AA70" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB70" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC70" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6020,7 +6017,7 @@
         <v>89</v>
       </c>
       <c r="C71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D71" t="s">
         <v>90</v>
@@ -6077,7 +6074,7 @@
         <v>252</v>
       </c>
       <c r="W71" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="X71" t="s">
         <v>338</v>
@@ -6086,10 +6083,10 @@
         <v>341</v>
       </c>
       <c r="AA71" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB71" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC71" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6104,7 +6101,7 @@
         <v>207</v>
       </c>
       <c r="C72" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D72" t="s">
         <v>78</v>
@@ -6161,16 +6158,16 @@
         <v>280</v>
       </c>
       <c r="W72" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Z72" t="s">
         <v>341</v>
       </c>
       <c r="AA72" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB72" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC72" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6180,12 +6177,12 @@
       'sunday-start':"1000", 'sunday-end':"1800", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1400", 'friday-end':"1800", 'saturday-start':"1000", 'saturday-end':"1800"},  'description': " $1 off all drafts \n $3.50 Wells \n $5 grilled cheese meals.", 'link':"http://www.pourbrothers.com/", 'pricing':"medium",   'phone-number': "", 'address': "220 Linden Street, Fort Collins, CO 80524", 'other-amenities': ['','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="73" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>209</v>
       </c>
       <c r="C73" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D73" t="s">
         <v>303</v>
@@ -6206,10 +6203,10 @@
         <v>341</v>
       </c>
       <c r="AA73" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB73" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC73" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6219,12 +6216,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://prostbrewing.com/", 'pricing':"medium",   'phone-number': "", 'address': "321 Old Firehouse Alley, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="74" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>211</v>
       </c>
       <c r="C74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D74" t="s">
         <v>303</v>
@@ -6248,10 +6245,10 @@
         <v>342</v>
       </c>
       <c r="AA74" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB74" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC74" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6266,7 +6263,7 @@
         <v>172</v>
       </c>
       <c r="C75" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D75" t="s">
         <v>173</v>
@@ -6317,16 +6314,16 @@
         <v>269</v>
       </c>
       <c r="W75" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Z75" t="s">
         <v>341</v>
       </c>
       <c r="AA75" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB75" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC75" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6341,7 +6338,7 @@
         <v>43</v>
       </c>
       <c r="C76" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D76" t="s">
         <v>44</v>
@@ -6392,10 +6389,10 @@
         <v>341</v>
       </c>
       <c r="AA76" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB76" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC76" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6405,12 +6402,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.riograndemexican.com/", 'pricing':"medium",   'phone-number': "", 'address': "143 W Mountain Ave, Fort Collins 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="77" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>213</v>
       </c>
       <c r="C77" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D77" t="s">
         <v>214</v>
@@ -6422,7 +6419,7 @@
         <v>215</v>
       </c>
       <c r="W77" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="X77" t="s">
         <v>338</v>
@@ -6431,10 +6428,10 @@
         <v>28</v>
       </c>
       <c r="AA77" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB77" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC77" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6444,12 +6441,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.road34.com/", 'pricing':"medium",   'phone-number': "", 'address': "1213 W. Elizabeth Street, Fort Collins, CO 80521", 'other-amenities': ['outdoor','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="78" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D78" t="s">
         <v>60</v>
@@ -6467,10 +6464,10 @@
         <v>341</v>
       </c>
       <c r="AA78" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB78" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC78" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6480,12 +6477,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.rodiziogrill.com/fort-collins/", 'pricing':"high",   'phone-number': "", 'address': "200 Jefferson St, Fort Collins 80524", 'other-amenities': ['','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="79" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>216</v>
       </c>
       <c r="C79" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D79" t="s">
         <v>217</v>
@@ -6497,16 +6494,16 @@
         <v>218</v>
       </c>
       <c r="W79" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Z79" t="s">
         <v>341</v>
       </c>
       <c r="AA79" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB79" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC79" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6516,33 +6513,33 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.scrumpys.net", 'pricing':"medium",   'phone-number': "", 'address': " 215 N. College Avenue, Fort Collins, CO 80524", 'other-amenities': ['','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="80" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
+        <v>453</v>
+      </c>
+      <c r="C80" t="s">
+        <v>351</v>
+      </c>
+      <c r="D80" t="s">
         <v>454</v>
-      </c>
-      <c r="C80" t="s">
-        <v>352</v>
-      </c>
-      <c r="D80" t="s">
-        <v>455</v>
       </c>
       <c r="E80" t="s">
         <v>54</v>
       </c>
       <c r="G80" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="W80" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="Z80" t="s">
         <v>28</v>
       </c>
       <c r="AA80" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB80" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC80" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6552,12 +6549,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.slycepizzaco.com/", 'pricing':"low",   'phone-number': "", 'address': "163 W. Mountain Ave, Fort Collins, Co 80524", 'other-amenities': ['','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="81" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C81" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D81" t="s">
         <v>93</v>
@@ -6566,7 +6563,7 @@
         <v>28</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H81">
         <v>1100</v>
@@ -6605,10 +6602,10 @@
         <v>1800</v>
       </c>
       <c r="V81" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="W81" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="X81" t="s">
         <v>338</v>
@@ -6617,10 +6614,10 @@
         <v>342</v>
       </c>
       <c r="AA81" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB81" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC81" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6635,7 +6632,7 @@
         <v>219</v>
       </c>
       <c r="C82" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D82" t="s">
         <v>303</v>
@@ -6647,7 +6644,7 @@
         <v>220</v>
       </c>
       <c r="W82" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="X82" t="s">
         <v>338</v>
@@ -6659,10 +6656,10 @@
         <v>342</v>
       </c>
       <c r="AA82" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB82" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC82" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6677,7 +6674,7 @@
         <v>325</v>
       </c>
       <c r="C83" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D83" t="s">
         <v>226</v>
@@ -6734,16 +6731,16 @@
         <v>326</v>
       </c>
       <c r="W83" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Z83" t="s">
         <v>341</v>
       </c>
       <c r="AA83" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB83" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC83" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6753,12 +6750,12 @@
       'sunday-start':"1600", 'sunday-end':"1800", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"2400", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "$3 – $6 drink and food specials", 'link':"http://www.socialfortcollins.com/", 'pricing':"high",   'phone-number': "", 'address': "1, Old Town Square #7, Fort Collins, CO 80524", 'other-amenities': ['','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="84" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>103</v>
       </c>
       <c r="C84" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D84" t="s">
         <v>104</v>
@@ -6770,16 +6767,16 @@
         <v>105</v>
       </c>
       <c r="W84" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Z84" t="s">
         <v>341</v>
       </c>
       <c r="AA84" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB84" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC84" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6789,12 +6786,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.sonnylubicksteakhouse.com", 'pricing':"high",   'phone-number': "", 'address': "115 S College Ave, Fort Collins 80524", 'other-amenities': ['','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="85" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>137</v>
       </c>
       <c r="C85" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D85" t="s">
         <v>138</v>
@@ -6812,10 +6809,10 @@
         <v>341</v>
       </c>
       <c r="AA85" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB85" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC85" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6825,12 +6822,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://espoons.com", 'pricing':"low",   'phone-number': "", 'address': "172 N College Ave, Fort Collins 80524", 'other-amenities': ['','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="86" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>118</v>
       </c>
       <c r="C86" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D86" t="s">
         <v>119</v>
@@ -6842,16 +6839,16 @@
         <v>120</v>
       </c>
       <c r="W86" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="Z86" t="s">
         <v>342</v>
       </c>
       <c r="AA86" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB86" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC86" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6866,7 +6863,7 @@
         <v>40</v>
       </c>
       <c r="C87" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D87" t="s">
         <v>41</v>
@@ -6887,10 +6884,10 @@
         <v>28</v>
       </c>
       <c r="AA87" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB87" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC87" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6905,7 +6902,7 @@
         <v>37</v>
       </c>
       <c r="C88" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D88" t="s">
         <v>38</v>
@@ -6968,10 +6965,10 @@
         <v>28</v>
       </c>
       <c r="AA88" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB88" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC88" s="4" t="str">
         <f t="shared" si="1"/>
@@ -6981,30 +6978,30 @@
       'sunday-start':"1130", 'sunday-end':"1400", 'monday-start':"1100", 'monday-end':"1400", 'tuesday-start':"1100", 'tuesday-end':"1400", 'wednesday-start':"1100", 'wednesday-end':"1400", 'thursday-start':"1100", 'thursday-end':"1400", 'friday-start':"1100", 'friday-end':"1400", 'saturday-start':"1130", 'saturday-end':"1400"},  'description': "Special Priced Lunch Menu", 'link':"http://suhsushi.wixsite.com/suhsushi", 'pricing':"medium",   'phone-number': "", 'address': "200 W Prospect Rd, Fort Collins 80526", 'other-amenities': ['','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="89" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C89" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D89" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E89" t="s">
         <v>28</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="W89" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AA89" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB89" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC89" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7019,7 +7016,7 @@
         <v>112</v>
       </c>
       <c r="C90" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D90" t="s">
         <v>113</v>
@@ -7061,16 +7058,16 @@
         <v>1800</v>
       </c>
       <c r="W90" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="Z90" t="s">
         <v>28</v>
       </c>
       <c r="AA90" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB90" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC90" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7080,12 +7077,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1700", 'monday-end':"1800", 'tuesday-start':"1700", 'tuesday-end':"1800", 'wednesday-start':"1700", 'wednesday-end':"1800", 'thursday-start':"1700", 'thursday-end':"1800", 'friday-start':"1700", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.tajmahalfortcollins.com/", 'pricing':"medium",   'phone-number': "", 'address': "148 W Oak St, Fort Collins 80524", 'other-amenities': ['','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="91" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>80</v>
       </c>
       <c r="C91" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D91" t="s">
         <v>81</v>
@@ -7097,7 +7094,7 @@
         <v>82</v>
       </c>
       <c r="W91" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="X91" t="s">
         <v>338</v>
@@ -7106,10 +7103,10 @@
         <v>341</v>
       </c>
       <c r="AA91" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB91" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC91" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7119,12 +7116,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.tastyharmony.com/", 'pricing':"medium",   'phone-number': "", 'address': "130 South Mason, Fort Collins 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="92" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>100</v>
       </c>
       <c r="C92" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D92" t="s">
         <v>101</v>
@@ -7136,16 +7133,16 @@
         <v>102</v>
       </c>
       <c r="W92" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="Z92" t="s">
         <v>342</v>
       </c>
       <c r="AA92" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB92" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC92" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7155,12 +7152,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.thaipepperco.com", 'pricing':"low",   'phone-number': "", 'address': "109 E Laurel St, Fort Collins 80524", 'other-amenities': ['','','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="93" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>83</v>
       </c>
       <c r="C93" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D93" t="s">
         <v>84</v>
@@ -7181,10 +7178,10 @@
         <v>28</v>
       </c>
       <c r="AA93" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB93" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC93" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7194,12 +7191,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.thefourfifteen.com/", 'pricing':"high",   'phone-number': "", 'address': "415 S Mason, Fort Collins 80521", 'other-amenities': ['outdoor','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="94" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:29" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>221</v>
       </c>
       <c r="C94" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D94" t="s">
         <v>90</v>
@@ -7244,16 +7241,16 @@
         <v>283</v>
       </c>
       <c r="W94" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="Z94" t="s">
         <v>28</v>
       </c>
       <c r="AA94" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB94" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC94" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7263,12 +7260,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "Drinks \n $2 Domestics &amp; Well Drinks \n $3 Flavored Pinnacle &amp; Three Olives Vodka \n $4 Mile High Spirits \n Fireside &amp; Fireside Peach Bourbon, Elevate Vodka, Denver Dry Gin, Peg Leg Rum \n $1 off Craft Drafts \n Food \n $2.50 Pork Sammys \n $3 Poutine", 'link':"http://www.thecoloradoroom.com", 'pricing':"medium",   'phone-number': "", 'address': "642 S. College Ave, Fort Collins, CO 80524", 'other-amenities': ['','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="95" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>175</v>
       </c>
       <c r="C95" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D95" t="s">
         <v>176</v>
@@ -7319,10 +7316,10 @@
         <v>341</v>
       </c>
       <c r="AA95" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB95" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC95" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7337,7 +7334,7 @@
         <v>223</v>
       </c>
       <c r="C96" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D96" t="s">
         <v>303</v>
@@ -7376,16 +7373,16 @@
         <v>284</v>
       </c>
       <c r="W96" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Z96" t="s">
         <v>28</v>
       </c>
       <c r="AA96" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB96" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC96" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7395,12 +7392,12 @@
       'sunday-start':"1800", 'sunday-end':"2400", 'monday-start':"", 'monday-end':"", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "$1 off guest drafts", 'link':"http://www.threefourbeerco.com/", 'pricing':"medium",   'phone-number': "", 'address': "829 S. Shields Street, #100, Fort Collins, CO 80521", 'other-amenities': ['','','medium'], 'has-drink':true, 'has-food':false},</v>
       </c>
     </row>
-    <row r="97" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:29" ht="174" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>225</v>
       </c>
       <c r="C97" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D97" t="s">
         <v>226</v>
@@ -7466,10 +7463,10 @@
         <v>341</v>
       </c>
       <c r="AA97" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB97" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC97" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7479,21 +7476,21 @@
       'sunday-start':"930", 'sunday-end':"2400", 'monday-start':"1030", 'monday-end':"1900", 'tuesday-start':"1030", 'tuesday-end':"1900", 'wednesday-start':"1030", 'wednesday-end':"1900", 'thursday-start':"1030", 'thursday-end':"1900", 'friday-start':"1030", 'friday-end':"1900", 'saturday-start':"930", 'saturday-end':"1900"},  'description': "Free pool during Happy Hour and all day Tuesday \n $2.00 Domestic Drafts \n $3.00 Select Micro Drafts \n $3.00 Single/$5.00 Double Wells and Freshies \n $5.00 Moscow Mules \n Happy Hour Appetizers: $6.00 Select appetizers Monday thru Friday 2 PM til 6 PM", 'link':"https://tonysbarfortcollins.com/", 'pricing':"medium",   'phone-number': "", 'address': "224 S. College Avenue, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','hard'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="98" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:29" ht="145" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C98" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D98" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E98" t="s">
         <v>28</v>
       </c>
       <c r="G98" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J98">
         <v>1500</v>
@@ -7526,10 +7523,10 @@
         <v>1900</v>
       </c>
       <c r="V98" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="W98" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="X98" t="s">
         <v>338</v>
@@ -7538,10 +7535,10 @@
         <v>342</v>
       </c>
       <c r="AA98" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AB98" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AC98" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7551,12 +7548,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1900", 'tuesday-start':"1500", 'tuesday-end':"1900", 'wednesday-start':"1500", 'wednesday-end':"1900", 'thursday-start':"1500", 'thursday-end':"1900", 'friday-start':"1500", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "$1.50 Off All Beers and Margs \n $0.50 Off Everything Else", 'link':"https://torchystacos.com/location/fort-collins/", 'pricing':"medium",   'phone-number': "", 'address': "3280 S COLLEGE AVE FORT COLLINS, CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
     </row>
-    <row r="99" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>228</v>
       </c>
       <c r="C99" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D99" t="s">
         <v>53</v>
@@ -7568,16 +7565,16 @@
         <v>229</v>
       </c>
       <c r="W99" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Z99" t="s">
         <v>342</v>
       </c>
       <c r="AA99" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB99" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC99" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7587,12 +7584,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"http://www.tortillamarissas.com", 'pricing':"medium",   'phone-number': "", 'address': "2635 S. College Avenue, Fort Collins, CO 80525", 'other-amenities': ['','','easy'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="100" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:29" ht="203" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>327</v>
       </c>
       <c r="C100" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D100" t="s">
         <v>328</v>
@@ -7649,16 +7646,16 @@
         <v>329</v>
       </c>
       <c r="W100" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Z100" t="s">
         <v>341</v>
       </c>
       <c r="AA100" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB100" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC100" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7668,21 +7665,21 @@
       'sunday-start':"1100", 'sunday-end':"1900", 'monday-start':"1100", 'monday-end':"2400", 'tuesday-start':"1100", 'tuesday-end':"2300", 'wednesday-start':"1100", 'wednesday-end':"2400", 'thursday-start':"1100", 'thursday-end':"2400", 'friday-start':"1100", 'friday-end':"1900", 'saturday-start':"1100", 'saturday-end':"1900"},  'description': "Monday-Sunday 11 am-7 pm: \n $2 domestics and $6 pitchers \n $2.50-micros and $8 pitchers \n $2 wells \n $2 PBR pints (all day) \n Monday: \n Happy Hour All Day \n Tuesday: \n 2-for-1 burgers 7pm-11pm \n $2 select micros 7pm-close \n Wednesday 7 pm-close: \n $2.50 New Belgium \n Thursday 7 pm-close: \n $2.50 Odell beers \n $1 tacos 6-11 pm \n Friday: \n $6 PBR pitchers and $2.50 Jagermeister \n Saturday: \n $4 domestic beer and brat \n Sunday: \n $16 wings and pitcher (domestic) \n $19 wings and pitcher (micro)", 'link':"http://www.trailheadtavern.com/", 'pricing':"low",   'phone-number': "", 'address': "148 W Mountain Ave, Fort Collins, CO 80524", 'other-amenities': ['','','hard'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="101" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
+        <v>457</v>
+      </c>
+      <c r="C101" t="s">
+        <v>351</v>
+      </c>
+      <c r="D101" t="s">
+        <v>423</v>
+      </c>
+      <c r="E101" t="s">
+        <v>28</v>
+      </c>
+      <c r="W101" t="s">
         <v>458</v>
-      </c>
-      <c r="C101" t="s">
-        <v>352</v>
-      </c>
-      <c r="D101" t="s">
-        <v>424</v>
-      </c>
-      <c r="E101" t="s">
-        <v>28</v>
-      </c>
-      <c r="W101" t="s">
-        <v>459</v>
       </c>
       <c r="X101" t="s">
         <v>338</v>
@@ -7691,10 +7688,10 @@
         <v>28</v>
       </c>
       <c r="AA101" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB101" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC101" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7709,7 +7706,7 @@
         <v>128</v>
       </c>
       <c r="C102" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D102" t="s">
         <v>129</v>
@@ -7721,7 +7718,7 @@
         <v>130</v>
       </c>
       <c r="W102" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="X102" t="s">
         <v>338</v>
@@ -7730,10 +7727,10 @@
         <v>28</v>
       </c>
       <c r="AA102" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB102" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC102" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7748,7 +7745,7 @@
         <v>230</v>
       </c>
       <c r="C103" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D103" t="s">
         <v>147</v>
@@ -7766,10 +7763,10 @@
         <v>28</v>
       </c>
       <c r="AA103" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB103" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC103" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7779,12 +7776,12 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"https://www.wolverinefarm.org/letterpressandpublickhouse/", 'pricing':"medium",   'phone-number': "", 'address': "316 Willow Street, Fort Collins, CO 80524", 'other-amenities': ['','','medium'], 'has-drink':false, 'has-food':false},</v>
       </c>
     </row>
-    <row r="104" spans="2:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:29" ht="116" x14ac:dyDescent="0.35">
       <c r="B104" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C104" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D104" t="s">
         <v>50</v>
@@ -7802,10 +7799,10 @@
         <v>342</v>
       </c>
       <c r="AA104" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB104" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC104" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7820,7 +7817,7 @@
         <v>232</v>
       </c>
       <c r="C105" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D105" t="s">
         <v>303</v>
@@ -7832,7 +7829,7 @@
         <v>233</v>
       </c>
       <c r="W105" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="X105" t="s">
         <v>338</v>
@@ -7844,10 +7841,10 @@
         <v>28</v>
       </c>
       <c r="AA105" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AB105" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AC105" s="4" t="str">
         <f t="shared" si="1"/>
@@ -7929,5 +7926,6 @@
     <hyperlink ref="W43" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>